<commit_message>
EPBDS-10072 introduce new keyword for all business enumeration properties in file name processor
--HG--
branch : EPBDS-10072
</commit_message>
<xml_diff>
--- a/Util/openl-project-archetype/resources/archetype-resources/src/test/openl/rules/Tests.xlsx
+++ b/Util/openl-project-archetype/resources/archetype-resources/src/test/openl/rules/Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-project-archetype\resources\META-INF\maven\archetype-resources\src\test\openl\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\Util\openl-project-archetype\resources\archetype-resources\src\test\openl\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BAB3EC-6336-49AD-ACC0-7CEB01721F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271CB77B-B5DF-469A-AD5E-6EF30C942DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Hello, John Smith!</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <r>
@@ -64,6 +67,26 @@
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SayHello</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
@@ -71,11 +94,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SayHello</t>
+      <t>SayHelloTest</t>
     </r>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -173,10 +193,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -460,7 +480,7 @@
   <dimension ref="C3:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,10 +490,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
@@ -485,7 +505,7 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
@@ -505,8 +525,8 @@
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>